<commit_message>
Add LIPID MAPS converter with CLI commands
</commit_message>
<xml_diff>
--- a/Test/TestInput/test_crosscheck.xlsx
+++ b/Test/TestInput/test_crosscheck.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC8904C-65F1-453E-A576-A0003EB99260}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E3AD24-87EB-4165-A1E8-F0C444AFDB6C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19875" yWindow="8940" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14355" yWindow="1575" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="208">
   <si>
     <t>16:0p/HETE-PE</t>
   </si>
@@ -629,6 +629,27 @@
   </si>
   <si>
     <t>FA22:5[5xDB,2xOH]</t>
+  </si>
+  <si>
+    <t>16:0</t>
+  </si>
+  <si>
+    <t>20:2(10Z,13E)(9Ke,15OH[S])</t>
+  </si>
+  <si>
+    <t>BAD_Test1</t>
+  </si>
+  <si>
+    <t>BAD_Test2</t>
+  </si>
+  <si>
+    <t>BAD_Test3</t>
+  </si>
+  <si>
+    <t>BAD_Test4</t>
+  </si>
+  <si>
+    <t>BAD_Test5</t>
   </si>
 </sst>
 </file>
@@ -664,8 +685,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +980,7 @@
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,7 +996,7 @@
       <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -991,8 +1013,8 @@
       <c r="D2" t="s">
         <v>189</v>
       </c>
-      <c r="E2" t="s">
-        <v>115</v>
+      <c r="E2" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1008,8 +1030,8 @@
       <c r="D3" t="s">
         <v>190</v>
       </c>
-      <c r="E3" t="s">
-        <v>116</v>
+      <c r="E3" s="1" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1025,8 +1047,8 @@
       <c r="D4" t="s">
         <v>191</v>
       </c>
-      <c r="E4" t="s">
-        <v>141</v>
+      <c r="E4" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1042,8 +1064,8 @@
       <c r="D5" t="s">
         <v>192</v>
       </c>
-      <c r="E5" t="s">
-        <v>147</v>
+      <c r="E5" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1059,8 +1081,8 @@
       <c r="D6" t="s">
         <v>193</v>
       </c>
-      <c r="E6" t="s">
-        <v>142</v>
+      <c r="E6" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1076,8 +1098,8 @@
       <c r="D7" t="s">
         <v>194</v>
       </c>
-      <c r="E7" t="s">
-        <v>148</v>
+      <c r="E7" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1093,8 +1115,8 @@
       <c r="D8" t="s">
         <v>103</v>
       </c>
-      <c r="E8" t="s">
-        <v>143</v>
+      <c r="E8" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1110,8 +1132,8 @@
       <c r="D9" t="s">
         <v>104</v>
       </c>
-      <c r="E9" t="s">
-        <v>149</v>
+      <c r="E9" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1127,8 +1149,8 @@
       <c r="D10" t="s">
         <v>105</v>
       </c>
-      <c r="E10" t="s">
-        <v>144</v>
+      <c r="E10" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1144,8 +1166,8 @@
       <c r="D11" t="s">
         <v>106</v>
       </c>
-      <c r="E11" t="s">
-        <v>150</v>
+      <c r="E11" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1161,8 +1183,8 @@
       <c r="D12" t="s">
         <v>107</v>
       </c>
-      <c r="E12" t="s">
-        <v>145</v>
+      <c r="E12" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1178,8 +1200,8 @@
       <c r="D13" t="s">
         <v>108</v>
       </c>
-      <c r="E13" t="s">
-        <v>151</v>
+      <c r="E13" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1195,8 +1217,8 @@
       <c r="D14" t="s">
         <v>109</v>
       </c>
-      <c r="E14" t="s">
-        <v>146</v>
+      <c r="E14" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1212,8 +1234,8 @@
       <c r="D15" t="s">
         <v>110</v>
       </c>
-      <c r="E15" t="s">
-        <v>152</v>
+      <c r="E15" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1229,8 +1251,11 @@
       <c r="D16" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1243,8 +1268,11 @@
       <c r="D17" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1257,8 +1285,11 @@
       <c r="D18" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1272,7 +1303,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1286,7 +1317,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1300,7 +1331,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1314,7 +1345,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1328,7 +1359,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1342,7 +1373,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1356,7 +1387,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1370,7 +1401,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1384,7 +1415,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1398,7 +1429,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1412,7 +1443,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1426,7 +1457,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1440,7 +1471,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1615,6 +1646,12 @@
       <c r="B44" t="s">
         <v>89</v>
       </c>
+      <c r="C44" t="s">
+        <v>205</v>
+      </c>
+      <c r="D44" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1678,6 +1715,14 @@
       </c>
       <c r="B52" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>203</v>
+      </c>
+      <c r="B53" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add unittest for convLION, update README.md
</commit_message>
<xml_diff>
--- a/Test/TestInput/test_crosscheck.xlsx
+++ b/Test/TestInput/test_crosscheck.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E3AD24-87EB-4165-A1E8-F0C444AFDB6C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D24469-5087-4CDD-B198-C6697E64024E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14355" yWindow="1575" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="210">
   <si>
     <t>16:0p/HETE-PE</t>
   </si>
@@ -640,24 +640,38 @@
     <t>BAD_Test1</t>
   </si>
   <si>
-    <t>BAD_Test2</t>
-  </si>
-  <si>
-    <t>BAD_Test3</t>
-  </si>
-  <si>
-    <t>BAD_Test4</t>
-  </si>
-  <si>
-    <t>BAD_Test5</t>
+    <t>BAD_ID_Test</t>
+  </si>
+  <si>
+    <t>16_0</t>
+  </si>
+  <si>
+    <t>HDotHE</t>
+  </si>
+  <si>
+    <t>OE(16:0/20:4(10-OH))</t>
+  </si>
+  <si>
+    <t>18:1</t>
+  </si>
+  <si>
+    <t>20:4(5Z,9E,11Z,14Z)(8Ke)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -685,9 +699,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,39 +990,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="36.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1016,8 +1042,11 @@
       <c r="E2" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1031,10 +1060,13 @@
         <v>190</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1048,10 +1080,13 @@
         <v>191</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1065,10 +1100,13 @@
         <v>192</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1082,10 +1120,10 @@
         <v>193</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1099,10 +1137,10 @@
         <v>194</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1116,10 +1154,10 @@
         <v>103</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1133,10 +1171,10 @@
         <v>104</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -1150,10 +1188,10 @@
         <v>105</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1167,10 +1205,10 @@
         <v>106</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1184,10 +1222,10 @@
         <v>107</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -1201,10 +1239,10 @@
         <v>108</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -1218,10 +1256,10 @@
         <v>109</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1235,10 +1273,10 @@
         <v>110</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1252,7 +1290,7 @@
         <v>111</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1269,7 +1307,7 @@
         <v>112</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1285,8 +1323,8 @@
       <c r="D18" t="s">
         <v>113</v>
       </c>
-      <c r="E18" t="s">
-        <v>207</v>
+      <c r="E18" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1302,6 +1340,9 @@
       <c r="D19" t="s">
         <v>114</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1646,12 +1687,6 @@
       <c r="B44" t="s">
         <v>89</v>
       </c>
-      <c r="C44" t="s">
-        <v>205</v>
-      </c>
-      <c r="D44" t="s">
-        <v>206</v>
-      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1715,14 +1750,6 @@
       </c>
       <c r="B52" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>203</v>
-      </c>
-      <c r="B53" t="s">
-        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>